<commit_message>
add rolling target rank and target % to all historical
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/pnl_tables.xlsx
+++ b/resultsAnalysis/data_warehouse/pnl_tables.xlsx
@@ -72,6 +72,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -803,6 +804,44 @@
         <a:xfrm>
           <a:off x="24765000" y="2857500"/>
           <a:ext cx="8026400" cy="2362200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="49530000" y="2857500"/>
+          <a:ext cx="8026400" cy="2336800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1341,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AH31" sqref="AH31"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BN9" sqref="BN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>